<commit_message>
Fixed the version number
</commit_message>
<xml_diff>
--- a/InputFiles/Parameters Datasheet.xlsx
+++ b/InputFiles/Parameters Datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078E4141-E670-4E37-AE57-E2FCA42DAFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE2C727-D2A1-4FCB-B633-921A87F15ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -43,12 +43,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="133">
   <si>
     <t>SCWAD</t>
-  </si>
-  <si>
-    <t>v0.0.4</t>
   </si>
   <si>
     <t>Distribution Types</t>
@@ -2451,7 +2448,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2460,8 +2457,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2492,46 +2489,46 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1">
         <v>1.98</v>
@@ -2545,16 +2542,16 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="11">
         <v>58</v>
@@ -2568,16 +2565,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>104</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="11">
         <v>288</v>
@@ -2591,16 +2588,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>106</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="11">
         <v>29</v>
@@ -2614,16 +2611,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>108</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="11">
         <v>15</v>
@@ -2635,16 +2632,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="11">
         <v>8</v>
@@ -2656,16 +2653,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="11">
         <v>147</v>
@@ -2679,16 +2676,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="11">
         <v>172</v>
@@ -2702,16 +2699,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="11">
         <v>86</v>
@@ -2725,16 +2722,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="11">
         <v>102</v>
@@ -2748,16 +2745,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" s="11">
         <v>124</v>
@@ -2771,16 +2768,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" s="11">
         <v>170</v>
@@ -2794,16 +2791,16 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="11">
         <v>235.42</v>
@@ -2815,16 +2812,16 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="11">
         <v>238</v>
@@ -2836,16 +2833,16 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="11">
         <v>66</v>
@@ -2859,16 +2856,16 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="11">
         <v>79</v>
@@ -2882,16 +2879,16 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="11">
         <v>88</v>
@@ -2905,16 +2902,16 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="11">
         <v>19</v>
@@ -2928,16 +2925,16 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" s="11">
         <v>155</v>
@@ -2949,16 +2946,16 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="E21" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" s="11">
         <v>0.14271105710000001</v>
@@ -2972,16 +2969,16 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" s="11">
         <v>3322</v>
@@ -2993,16 +2990,16 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" s="11">
         <v>3023.8</v>
@@ -3014,16 +3011,16 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" s="11">
         <v>1897.68</v>
@@ -3035,16 +3032,16 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="11">
         <v>260.08999999999997</v>
@@ -3056,16 +3053,16 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" s="11">
         <v>1007.082</v>
@@ -3077,16 +3074,16 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>131</v>
-      </c>
       <c r="E27" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" s="14">
         <v>231</v>
@@ -3125,7 +3122,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -3137,15 +3134,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3153,7 +3150,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -3161,7 +3158,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3169,7 +3166,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -3177,7 +3174,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3185,7 +3182,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3210,27 +3207,27 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3248,7 +3245,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3257,7 +3254,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3266,7 +3263,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3275,7 +3272,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3283,12 +3280,12 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3296,17 +3293,17 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3314,27 +3311,27 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3363,7 +3360,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3382,46 +3379,46 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -3433,16 +3430,16 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="E3" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="14">
         <v>8</v>
@@ -3496,46 +3493,46 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -3547,16 +3544,16 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="11">
         <v>0</v>
@@ -3570,16 +3567,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="11">
         <v>2</v>
@@ -3593,16 +3590,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="11">
         <v>0</v>
@@ -3616,16 +3613,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="11">
         <v>4</v>
@@ -3637,16 +3634,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="11">
         <v>1</v>
@@ -3660,16 +3657,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>55</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="11">
         <v>50</v>
@@ -3681,16 +3678,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>57</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="11">
         <v>100</v>
@@ -3702,16 +3699,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="E10" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="11">
         <v>6</v>
@@ -3725,16 +3722,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="E11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="11">
         <v>6</v>
@@ -3748,16 +3745,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="E12" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" s="11">
         <v>0.3</v>
@@ -3771,16 +3768,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>63</v>
-      </c>
       <c r="E13" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11">
@@ -3796,16 +3793,16 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>65</v>
-      </c>
       <c r="E14" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="11">
         <v>6</v>
@@ -3817,16 +3814,16 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>67</v>
-      </c>
       <c r="E15" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F15" s="11">
         <v>0.93855472579518462</v>
@@ -3840,16 +3837,16 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="E16" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16" s="11">
         <v>0.74555164756008985</v>
@@ -3863,16 +3860,16 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="E17" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="11">
         <v>67</v>
@@ -3886,16 +3883,16 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="E18" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="14">
         <v>0.5</v>
@@ -3953,46 +3950,46 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -4006,16 +4003,16 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="11">
         <v>0</v>
@@ -4029,16 +4026,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="11">
         <v>1</v>
@@ -4052,16 +4049,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="11">
         <v>0</v>
@@ -4075,16 +4072,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="11">
         <v>0.5</v>
@@ -4096,16 +4093,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="11">
         <v>2.84</v>
@@ -4119,16 +4116,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="11">
         <v>0.33300000000000002</v>
@@ -4140,16 +4137,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>63</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11">
@@ -4165,16 +4162,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="E10" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="11">
         <v>1</v>
@@ -4186,16 +4183,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="E11" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" s="11">
         <v>0</v>
@@ -4207,16 +4204,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="E12" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="14">
         <v>3.55</v>
@@ -4270,46 +4267,46 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1">
         <v>3</v>
@@ -4323,16 +4320,16 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="11">
         <v>0.3</v>
@@ -4346,16 +4343,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="11">
         <v>3</v>
@@ -4369,16 +4366,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="11">
         <v>1</v>
@@ -4392,16 +4389,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="11">
         <v>1</v>
@@ -4413,16 +4410,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>82</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="11">
         <v>2</v>
@@ -4434,16 +4431,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="11">
         <v>4.5</v>
@@ -4455,16 +4452,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>63</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="11">
         <v>1.18</v>
@@ -4478,16 +4475,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="11">
         <v>7.4456000000000003E-6</v>
@@ -4501,16 +4498,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="E11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="11">
         <v>4.6443800000000002E-6</v>
@@ -4524,16 +4521,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="E12" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="11">
         <v>0</v>
@@ -4545,16 +4542,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>90</v>
-      </c>
       <c r="E13" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F13" s="11">
         <v>0.44063296134955682</v>
@@ -4568,16 +4565,16 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="E14" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F14" s="11">
         <v>0.35936935576071999</v>
@@ -4591,16 +4588,16 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>94</v>
-      </c>
       <c r="E15" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="11">
         <v>2.5000000000000001E-3</v>
@@ -4612,16 +4609,16 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="11">
         <v>1.6E-2</v>
@@ -4635,16 +4632,16 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="E17" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="11">
         <v>0</v>
@@ -4658,16 +4655,16 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F18" s="14">
         <v>2.1777681381292679</v>
@@ -4724,46 +4721,46 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
Two of the truncated normal distributions from EPA documentation don't have minimum values so I'm adding 0 for now so that they're read in correctly
</commit_message>
<xml_diff>
--- a/InputFiles/Parameters Datasheet.xlsx
+++ b/InputFiles/Parameters Datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE2C727-D2A1-4FCB-B633-921A87F15ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8AF11D-4206-40BC-9CF7-81983EEDCD46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -2472,7 +2472,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3122,7 +3122,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -3361,7 +3361,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,7 +3476,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E21" sqref="D21:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3779,7 +3779,9 @@
       <c r="E13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
       <c r="G13" s="11">
         <v>3</v>
       </c>
@@ -3931,8 +3933,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4148,7 +4150,9 @@
       <c r="E9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
       <c r="G9" s="11">
         <v>3</v>
       </c>
@@ -4251,7 +4255,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix some bugs related to parameter modification.
</commit_message>
<xml_diff>
--- a/InputFiles/Parameters Datasheet.xlsx
+++ b/InputFiles/Parameters Datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C967D95-BC74-446B-9DF7-5A65B5A54EE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8DC6F5-A8A0-4F7D-A043-E73CCF6016AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -781,318 +781,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1349,6 +1037,72 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1603,6 +1357,72 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1859,6 +1679,66 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -2085,6 +1965,66 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -2305,6 +2245,66 @@
           <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -2559,119 +2559,119 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Maximum" dataDxfId="88"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Mean/Mode" dataDxfId="87"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Standard Deviation" dataDxfId="86"/>
-    <tableColumn id="11" xr3:uid="{6D5D89BA-F5B6-48D7-8EB6-F84737897B28}" name="Lower Limit" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{48C3D1E7-422F-49D2-B091-B1AED1C3D586}" name="Upper Limit" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{C7F66B6D-AE49-4F19-BA50-224FF50E099F}" name="Step" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{6D5D89BA-F5B6-48D7-8EB6-F84737897B28}" name="Lower Limit" dataDxfId="85"/>
+    <tableColumn id="12" xr3:uid="{48C3D1E7-422F-49D2-B091-B1AED1C3D586}" name="Upper Limit" dataDxfId="84"/>
+    <tableColumn id="13" xr3:uid="{C7F66B6D-AE49-4F19-BA50-224FF50E099F}" name="Step" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:M18" totalsRowShown="0" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:M18" totalsRowShown="0" tableBorderDxfId="80">
   <autoFilter ref="A1:M18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="13">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Internal" dataDxfId="82"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{8EBBFD49-190C-4C2F-A6BC-0598AAC3E788}" name="Description" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Minimum" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Maximum" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Mean/Mode" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Standard Deviation" dataDxfId="73"/>
-    <tableColumn id="11" xr3:uid="{BD4375F0-63E9-45EC-BE2E-338374C10F8B}" name="Lower Limit" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{E3D45A75-803F-48B4-B112-11C4C63E6D6F}" name="Upper Limit" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{FFEC12A7-FD01-4D8C-85CF-A25BD15B0829}" name="Step" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Internal" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="77"/>
+    <tableColumn id="10" xr3:uid="{8EBBFD49-190C-4C2F-A6BC-0598AAC3E788}" name="Description" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Minimum" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Maximum" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Mean/Mode" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Standard Deviation" dataDxfId="70"/>
+    <tableColumn id="11" xr3:uid="{BD4375F0-63E9-45EC-BE2E-338374C10F8B}" name="Lower Limit" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{E3D45A75-803F-48B4-B112-11C4C63E6D6F}" name="Upper Limit" dataDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{FFEC12A7-FD01-4D8C-85CF-A25BD15B0829}" name="Step" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:M12" totalsRowShown="0" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:M12" totalsRowShown="0" tableBorderDxfId="64">
   <autoFilter ref="A1:M12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="13">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="69"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{2D3DA962-F373-48F5-BD94-00CC27106A46}" name="Description" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Minimum" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Maximum" dataDxfId="62"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Mean/Mode" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Standard Deviation" dataDxfId="60"/>
-    <tableColumn id="11" xr3:uid="{FF818C38-99D8-4486-B25F-2B94B62F77AF}" name="Lower Limit" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{8C44E4B8-6916-4798-9055-589FE4E4C903}" name="Upper Limit" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{8266E46A-7EC0-42D8-91D3-D2DC1B4352DE}" name="Step" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="61"/>
+    <tableColumn id="10" xr3:uid="{2D3DA962-F373-48F5-BD94-00CC27106A46}" name="Description" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Minimum" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Maximum" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Mean/Mode" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Standard Deviation" dataDxfId="54"/>
+    <tableColumn id="11" xr3:uid="{FF818C38-99D8-4486-B25F-2B94B62F77AF}" name="Lower Limit" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{8C44E4B8-6916-4798-9055-589FE4E4C903}" name="Upper Limit" dataDxfId="52"/>
+    <tableColumn id="13" xr3:uid="{8266E46A-7EC0-42D8-91D3-D2DC1B4352DE}" name="Step" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:M18" totalsRowShown="0" headerRowBorderDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:M18" totalsRowShown="0" headerRowBorderDxfId="48" tableBorderDxfId="47">
   <autoFilter ref="A1:M18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="13">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="55"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{A40104D1-3BF7-4068-8777-3D61F27973C1}" name="Description" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Minimum" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Maximum" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Mean/Mode" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Standard Deviation" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{83552614-5368-48EE-AE65-AA7B101E55EF}" name="Lower Limit" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{98998298-F4B1-4980-B79C-0BF0D0D59028}" name="Upper Limit" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{8E3814A1-C526-4157-B0D9-1258E47ACA45}" name="Step" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{A40104D1-3BF7-4068-8777-3D61F27973C1}" name="Description" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Minimum" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Maximum" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Mean/Mode" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Standard Deviation" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{83552614-5368-48EE-AE65-AA7B101E55EF}" name="Lower Limit" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{98998298-F4B1-4980-B79C-0BF0D0D59028}" name="Upper Limit" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{8E3814A1-C526-4157-B0D9-1258E47ACA45}" name="Step" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:M2" totalsRowShown="0" headerRowBorderDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:M2" totalsRowShown="0" headerRowBorderDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="13">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Internal" dataDxfId="41"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{4482773E-AA48-4795-9A9F-10283D12A976}" name="Description" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Minimum" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Maximum" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Mean/Mode" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Standard Deviation" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{0ED7EC4B-FD74-44E3-B1E6-428C431FDA88}" name="Lower Limit" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{4CA3754D-692A-40C0-BCC5-14D0E3AAF144}" name="Upper Limit" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{D4791B88-6435-44AE-9946-77D4E8CB6EA8}" name="Step" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Internal" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{4482773E-AA48-4795-9A9F-10283D12A976}" name="Description" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Minimum" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Maximum" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Mean/Mode" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Standard Deviation" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{0ED7EC4B-FD74-44E3-B1E6-428C431FDA88}" name="Lower Limit" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{4CA3754D-692A-40C0-BCC5-14D0E3AAF144}" name="Upper Limit" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{D4791B88-6435-44AE-9946-77D4E8CB6EA8}" name="Step" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:M27" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:M27" totalsRowShown="0" headerRowBorderDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A1:M27" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
     <sortCondition ref="B1:B2"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="27"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{3AFE3909-1CDD-46E0-8677-569A824534FB}" name="Description" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Minimum" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Maximum" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Mean/Mode" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Standard Deviation" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{3AFE3909-1CDD-46E0-8677-569A824534FB}" name="Description" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Minimum" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Maximum" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Mean/Mode" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Standard Deviation" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{08FFB9BF-C539-434A-A2F4-C19873D3AB3E}" name="Lower Limit" dataDxfId="2"/>
     <tableColumn id="12" xr3:uid="{CEDB540F-344B-4D49-8CD6-9F7746873840}" name="Upper Limit" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{4B3E9A2A-7D0A-4F2D-B694-DB4D2C83BA0A}" name="Step" dataDxfId="0"/>
@@ -3004,8 +3004,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3902,12 +3902,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J27">
-    <cfRule type="expression" dxfId="31" priority="27">
+    <cfRule type="expression" dxfId="16" priority="27">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J27">
-    <cfRule type="expression" dxfId="30" priority="28">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4319,8 +4319,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4729,7 +4729,7 @@
         <v>50</v>
       </c>
       <c r="M12" s="11">
-        <v>1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -4932,12 +4932,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J18">
-    <cfRule type="expression" dxfId="85" priority="15">
+    <cfRule type="expression" dxfId="82" priority="15">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J18">
-    <cfRule type="expression" dxfId="84" priority="32">
+    <cfRule type="expression" dxfId="81" priority="32">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5376,12 +5376,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J12">
-    <cfRule type="expression" dxfId="72" priority="18">
+    <cfRule type="expression" dxfId="66" priority="18">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J12">
-    <cfRule type="expression" dxfId="71" priority="31">
+    <cfRule type="expression" dxfId="65" priority="31">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6012,12 +6012,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J18">
-    <cfRule type="expression" dxfId="59" priority="21">
+    <cfRule type="expression" dxfId="50" priority="21">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J18">
-    <cfRule type="expression" dxfId="58" priority="30">
+    <cfRule type="expression" dxfId="49" priority="30">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6129,12 +6129,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J2">
-    <cfRule type="expression" dxfId="45" priority="24">
+    <cfRule type="expression" dxfId="33" priority="24">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J2">
-    <cfRule type="expression" dxfId="44" priority="29">
+    <cfRule type="expression" dxfId="32" priority="29">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>